<commit_message>
adicao pasta standing robot
</commit_message>
<xml_diff>
--- a/Sensor de temperatura/calculadora amp-op resistencia variavel.xlsx
+++ b/Sensor de temperatura/calculadora amp-op resistencia variavel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdb336c02ce1c635/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdb336c02ce1c635/Documentos/Github/Circuits/Sensor de temperatura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{B5796DF3-C5D5-4503-8E47-65C086B6E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4459408-0823-4C8E-8B60-66AD7A92ED3D}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{B5796DF3-C5D5-4503-8E47-65C086B6E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8475B818-CFC3-4B1C-AA67-5F84BD75E3F8}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2370" windowWidth="29040" windowHeight="17520" xr2:uid="{9CE5BA22-920D-4845-A281-257BCBBFBEFC}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{9CE5BA22-920D-4845-A281-257BCBBFBEFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>min</t>
   </si>
   <si>
-    <t>max</t>
-  </si>
-  <si>
     <t>DADOS</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>CALCULOS</t>
+  </si>
+  <si>
+    <t>ganh</t>
   </si>
 </sst>
 </file>
@@ -267,52 +267,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363547AB-FD45-4FA3-898B-9EA2B4C4A073}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,128 +661,128 @@
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="18"/>
+    <col min="7" max="7" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="H1" s="3" t="s">
+      <c r="C1" s="12"/>
+      <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="4"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5">
-        <v>1800</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="C2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
-        <v>270</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="C3" s="2">
+        <v>150</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="2">
         <f>0.5*10^-3</f>
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>5600</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="2">
         <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>5600</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="2">
         <f>4.477*10^-3</f>
         <v>4.4770000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <v>5000</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>22</v>
+      <c r="A9" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="10"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -793,7 +792,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="10"/>
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -803,67 +802,66 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-    </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="2" t="s">
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <f>I2-C13</f>
         <v>4.95</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <f>I2-C14</f>
         <v>2.5</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <f>(I2-I4)/I3-2/I5</f>
         <v>6553.2722805450076</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <f>(C6-C18)*(C5/C4)*(1+2*C3/C2)</f>
         <v>6.4999999999999766E-2</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <f>(C6-D18)*(C5/C4)*(1+2*C3/C2)</f>
         <v>3.25</v>
       </c>
-      <c r="G19" s="19"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>